<commit_message>
Bổ sung cột giá trước thuế
</commit_message>
<xml_diff>
--- a/Data/MaKho_MaVV.xlsx
+++ b/Data/MaKho_MaVV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_BB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{CD6DBDF0-90A9-4B69-BCA9-B102021F8FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF02DFD1-7B65-4925-BFC4-8066F32A132B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,7 +535,7 @@
   <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -577,16 +577,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>